<commit_message>
fix international projects test data
</commit_message>
<xml_diff>
--- a/assets/raw-data/international-projects/international_projects.xlsx
+++ b/assets/raw-data/international-projects/international_projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DrebenstedtN\mex-extractors\assets\raw-data\international-projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SchiebenhoeferH\projects\mex-extractors\assets\raw-data\international-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE03D82-6F31-4525-A385-8B19B4F227FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23E474-5D12-49A9-89BC-AE201B13B07B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1065" windowWidth="13485" windowHeight="5925" xr2:uid="{32DDDEEA-D3D1-44A9-AA05-C05A3ED86EE0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
   <si>
     <t>Project Abbreviation</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t>FG99</t>
+  </si>
+  <si>
+    <t>0000-1001</t>
+  </si>
+  <si>
+    <t>0000-1002</t>
+  </si>
+  <si>
+    <t>0000-1003</t>
+  </si>
+  <si>
+    <t>0000-1004</t>
+  </si>
+  <si>
+    <t>0000-1005</t>
+  </si>
+  <si>
+    <t>0000-1006</t>
   </si>
 </sst>
 </file>
@@ -860,10 +878,10 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1080,7 @@
         <v>94</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>30</v>
@@ -1104,7 +1122,7 @@
         <v>94</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>30</v>
@@ -1163,7 +1181,7 @@
         <v>97</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>30</v>
@@ -1210,7 +1228,7 @@
         <v>94</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>30</v>
@@ -1248,7 +1266,7 @@
         <v>94</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>30</v>
@@ -1302,7 +1320,7 @@
         <v>97</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Feature/mx 1583 make asset dependencies explicit (#103)
# PR Context
<!-- Additional info for the reviewer -->

Make dependent extractors explicitly dependent on each other.

# Changes
<!-- Changes in existing functionality -->

- make dependent extractors explicitly depend on each other (gippeweb on
confluence-vvt, biospecimen on synopse, odk on international-projects)

# Fixed
<!-- Fixed bugs -->

- fix confluence_vvt transformation: use interne Vorgangsnummer as
identifierInPrimarySource

---------

Signed-off-by: rababerladuseladim <rababerladuseladim@users.noreply.github.com>
Co-authored-by: Nicolas Drebenstedt <897972+cutoffthetop@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/raw-data/international-projects/international_projects.xlsx
+++ b/assets/raw-data/international-projects/international_projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DrebenstedtN\mex-extractors\assets\raw-data\international-projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SchiebenhoeferH\projects\mex-extractors\assets\raw-data\international-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE03D82-6F31-4525-A385-8B19B4F227FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23E474-5D12-49A9-89BC-AE201B13B07B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1065" windowWidth="13485" windowHeight="5925" xr2:uid="{32DDDEEA-D3D1-44A9-AA05-C05A3ED86EE0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="104">
   <si>
     <t>Project Abbreviation</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t>FG99</t>
+  </si>
+  <si>
+    <t>0000-1001</t>
+  </si>
+  <si>
+    <t>0000-1002</t>
+  </si>
+  <si>
+    <t>0000-1003</t>
+  </si>
+  <si>
+    <t>0000-1004</t>
+  </si>
+  <si>
+    <t>0000-1005</t>
+  </si>
+  <si>
+    <t>0000-1006</t>
   </si>
 </sst>
 </file>
@@ -860,10 +878,10 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1080,7 @@
         <v>94</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>30</v>
@@ -1104,7 +1122,7 @@
         <v>94</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>30</v>
@@ -1163,7 +1181,7 @@
         <v>97</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>30</v>
@@ -1210,7 +1228,7 @@
         <v>94</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="R7" s="4" t="s">
         <v>30</v>
@@ -1248,7 +1266,7 @@
         <v>94</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>30</v>
@@ -1302,7 +1320,7 @@
         <v>97</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>30</v>

</xml_diff>